<commit_message>
Just a little more . . .
</commit_message>
<xml_diff>
--- a/Web Tech Test Plan.xlsx
+++ b/Web Tech Test Plan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\school stuff\project3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\projects\project3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C400A8A-C128-4069-BEF3-CC4C06E4C783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A3D6F72-4D55-4E1A-A203-515DB26B15DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="October 15, 2023" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="36">
   <si>
     <t>Test case plan</t>
   </si>
@@ -118,9 +118,6 @@
     <t>Admin page works</t>
   </si>
   <si>
-    <t>The donut list can be edited from the admin page.</t>
-  </si>
-  <si>
     <t>Database</t>
   </si>
   <si>
@@ -128,6 +125,18 @@
   </si>
   <si>
     <t>The site can retrieve and edit data from the database.</t>
+  </si>
+  <si>
+    <t>The donut list can be edited from the admin page (creating, updating, and deleting donut listings).</t>
+  </si>
+  <si>
+    <t>Uzair</t>
+  </si>
+  <si>
+    <t>Have not begun work on CSS yet.</t>
+  </si>
+  <si>
+    <t>Have not added images yet.</t>
   </si>
 </sst>
 </file>
@@ -645,23 +654,23 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" customWidth="1"/>
-    <col min="4" max="4" width="35.5546875" customWidth="1"/>
-    <col min="5" max="5" width="28.109375" customWidth="1"/>
-    <col min="6" max="6" width="19.5546875" customWidth="1"/>
-    <col min="7" max="7" width="16.44140625" customWidth="1"/>
-    <col min="8" max="8" width="15.109375" customWidth="1"/>
-    <col min="9" max="9" width="19.88671875" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" customWidth="1"/>
+    <col min="4" max="4" width="35.5703125" customWidth="1"/>
+    <col min="5" max="5" width="28.140625" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" customWidth="1"/>
+    <col min="9" max="9" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -674,7 +683,7 @@
       <c r="H1" s="9"/>
       <c r="I1" s="9"/>
     </row>
-    <row r="2" spans="1:9" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10">
         <v>45212</v>
       </c>
@@ -687,7 +696,7 @@
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
     </row>
-    <row r="3" spans="1:9" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" s="1" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -716,7 +725,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -729,20 +738,23 @@
       <c r="D4" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="E4" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="F4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -755,20 +767,23 @@
       <c r="D5" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="E5" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="F5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" s="2" customFormat="1" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="2" customFormat="1" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>3</v>
       </c>
@@ -782,7 +797,7 @@
         <v>26</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>7</v>
@@ -790,11 +805,11 @@
       <c r="H6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" s="2" customFormat="1" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I6" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="2" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>4</v>
       </c>
@@ -805,41 +820,65 @@
         <v>28</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:9" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:9" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:9" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:9" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:9" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:9" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:9" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="17" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="18" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="19" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="20" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="21" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="22" s="4" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="23" ht="24.9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="24" ht="24.9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="25" ht="24.9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="26" ht="24.9" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="F8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:9" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:9" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:9" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:9" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:9" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:9" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:9" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" s="4" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:I1"/>
@@ -857,20 +896,20 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.109375" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" customWidth="1"/>
-    <col min="4" max="4" width="35.5546875" customWidth="1"/>
-    <col min="5" max="5" width="28.109375" customWidth="1"/>
-    <col min="6" max="6" width="19.5546875" customWidth="1"/>
-    <col min="7" max="7" width="16.44140625" customWidth="1"/>
-    <col min="8" max="8" width="15.109375" customWidth="1"/>
-    <col min="9" max="9" width="19.88671875" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" customWidth="1"/>
+    <col min="4" max="4" width="35.5703125" customWidth="1"/>
+    <col min="5" max="5" width="28.140625" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" customWidth="1"/>
+    <col min="9" max="9" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -883,7 +922,7 @@
       <c r="H1" s="9"/>
       <c r="I1" s="9"/>
     </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" s="2" customFormat="1" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10">
         <v>45216</v>
       </c>
@@ -896,7 +935,7 @@
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
     </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" s="2" customFormat="1" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -925,7 +964,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -951,7 +990,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -977,7 +1016,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>3</v>
       </c>
@@ -1006,19 +1045,19 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:9" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:9" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:9" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:9" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:9" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:9" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:9" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:9" s="4" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="17" ht="24.9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="18" ht="24.9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="19" ht="24.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:9" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:9" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:9" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:9" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:9" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:9" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:9" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:9" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:9" s="4" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:I1"/>

</xml_diff>